<commit_message>
CTPA-1179 more xsd! more xml! more xls!
</commit_message>
<xml_diff>
--- a/samplesvc-api/src/main/resources/excel/census-sample-blank.xlsx
+++ b/samplesvc-api/src/main/resources/excel/census-sample-blank.xlsx
@@ -175,16 +175,64 @@
           <xsd:pattern value="[\d ]{1,20}"/>
         </xsd:restriction>
       </xsd:simpleType>
+      <xsd:simpleType name="string_1_1">
+        <xsd:restriction base="xsd:string">
+          <xsd:minLength value="1"/>
+          <xsd:maxLength value="1"/>
+        </xsd:restriction>
+      </xsd:simpleType>
       <xsd:simpleType name="string_1_2">
         <xsd:restriction base="xsd:string">
           <xsd:minLength value="1"/>
           <xsd:maxLength value="2"/>
         </xsd:restriction>
       </xsd:simpleType>
+      <xsd:simpleType name="string_1_4">
+        <xsd:restriction base="xsd:string">
+          <xsd:minLength value="1"/>
+          <xsd:maxLength value="4"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+      <xsd:simpleType name="string_1_5">
+        <xsd:restriction base="xsd:string">
+          <xsd:minLength value="1"/>
+          <xsd:maxLength value="5"/>
+        </xsd:restriction>
+      </xsd:simpleType>
       <xsd:simpleType name="string_1_6">
         <xsd:restriction base="xsd:string">
           <xsd:minLength value="1"/>
           <xsd:maxLength value="6"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+      <xsd:simpleType name="string_1_7">
+        <xsd:restriction base="xsd:string">
+          <xsd:minLength value="1"/>
+          <xsd:maxLength value="7"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+      <xsd:simpleType name="string_1_8">
+        <xsd:restriction base="xsd:string">
+          <xsd:minLength value="1"/>
+          <xsd:maxLength value="8"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+      <xsd:simpleType name="string_1_10">
+        <xsd:restriction base="xsd:string">
+          <xsd:minLength value="1"/>
+          <xsd:maxLength value="10"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+      <xsd:simpleType name="string_1_12">
+        <xsd:restriction base="xsd:string">
+          <xsd:minLength value="1"/>
+          <xsd:maxLength value="12"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+      <xsd:simpleType name="string_1_13">
+        <xsd:restriction base="xsd:string">
+          <xsd:minLength value="1"/>
+          <xsd:maxLength value="13"/>
         </xsd:restriction>
       </xsd:simpleType>
       <xsd:simpleType name="string_1_20">
@@ -209,6 +257,11 @@
         <xsd:restriction base="xsd:string">
           <xsd:minLength value="0"/>
           <xsd:maxLength value="60"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+      <xsd:simpleType name="integer_1_4">
+        <xsd:restriction base="xsd:integer">
+          <xsd:pattern value="[\d]{1,4}"/>
         </xsd:restriction>
       </xsd:simpleType>
       <xsd:simpleType name="alphanum_1_9">
@@ -228,8 +281,8 @@
       <xsd:include schemaLocation="Schema2"/>
       <xsd:complexType name="SampleUnitBase">
         <xsd:sequence>
-          <xsd:element name="respondentRef" type="xsd:string" minOccurs="1" maxOccurs="1"/>
-          <xsd:element name="respondentType" minOccurs="1" maxOccurs="1">
+          <xsd:element name="sampleUnitRef" type="xsd:string" minOccurs="1" maxOccurs="1"/>
+          <xsd:element name="sampleUnitType" minOccurs="1" maxOccurs="1">
             <xsd:simpleType>
               <xsd:restriction base="xsd:string">
                 <xsd:enumeration value="H"/>
@@ -326,7 +379,7 @@
       </xsd:complexType>
     </xsd:schema>
   </Schema>
-  <Map ID="1" Name="censusSurveySample_Map" RootElement="censusSurveySample" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
+  <Map ID="2" Name="censusSurveySample_Map" RootElement="censusSurveySample" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true"/>
 </MapInfo>
 </file>
 
@@ -334,86 +387,86 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="A1:AA2" tableType="xml" insertRow="1" totalsRowShown="0">
   <autoFilter ref="A1:AA2"/>
   <tableColumns count="27">
-    <tableColumn id="1" uniqueName="respondentRef" name="respondentRef">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/respondentRef" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="2" uniqueName="respondentType" name="respondentType">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/respondentType" xmlDataType="string"/>
+    <tableColumn id="1" uniqueName="sampleUnitRef" name="respondentRef">
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/sampleUnitRef" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" uniqueName="sampleUnitType" name="respondentType">
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/sampleUnitType" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="treatmentRef" name="treatmentRef">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/treatmentRef" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/treatmentRef" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="line1" name="line1">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/line1" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/line1" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="5" uniqueName="line2" name="line2">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/line2" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/line2" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="6" uniqueName="line3" name="line3">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/line3" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/line3" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="7" uniqueName="line4" name="line4">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/line4" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/line4" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="8" uniqueName="line5" name="line5">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/line5" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/line5" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="9" uniqueName="postcode" name="postcode">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/postcode" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/postcode" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="10" uniqueName="title" name="title">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/title" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/title" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="11" uniqueName="forename" name="forename">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/forename" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/forename" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="12" uniqueName="surname" name="surname">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/surname" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/surname" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="13" uniqueName="phoneNumber" name="phoneNumber">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/phoneNumber" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/phoneNumber" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="14" uniqueName="emailAddress" name="emailAddress">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/emailAddress" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/emailAddress" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="15" uniqueName="addressType" name="addressType">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/addressType" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/addressType" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="16" uniqueName="estabType" name="estabType">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/estabType" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/estabType" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="17" uniqueName="organisationName" name="organisationName">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/organisationName" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/organisationName" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="18" uniqueName="category" name="category">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/category" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/category" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="19" uniqueName="ladCode" name="ladCode">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/ladCode" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/ladCode" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="20" uniqueName="latitude" name="latitude">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/latitude" xmlDataType="decimal"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/latitude" xmlDataType="decimal"/>
     </tableColumn>
     <tableColumn id="21" uniqueName="longitude" name="longitude">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/longitude" xmlDataType="decimal"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/longitude" xmlDataType="decimal"/>
     </tableColumn>
     <tableColumn id="22" uniqueName="htc" name="htc">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/htc" xmlDataType="int"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/htc" xmlDataType="int"/>
     </tableColumn>
     <tableColumn id="23" uniqueName="locality" name="locality">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/locality" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/locality" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="24" uniqueName="oa" name="oa">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/oa" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/oa" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="25" uniqueName="msoa" name="msoa">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/msoa" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/msoa" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="26" uniqueName="lsoa" name="lsoa">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/lsoa" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/lsoa" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="27" uniqueName="censusRegion" name="censusRegion">
-      <xmlColumnPr mapId="1" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/censusRegion" xmlDataType="string"/>
+      <xmlColumnPr mapId="2" xpath="/ns1:censusSurveySample/sampleUnits/censusSampleUnit/censusRegion" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -422,24 +475,24 @@
 
 <file path=xl/tables/tableSingleCells1.xml><?xml version="1.0" encoding="utf-8"?>
 <singleXmlCells xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <singleXmlCell id="5" r="B2" connectionId="0">
+  <singleXmlCell id="1" r="B2" connectionId="0">
     <xmlCellPr id="1" uniqueName="surveyRef">
-      <xmlPr mapId="1" xpath="/ns1:censusSurveySample/surveyRef" xmlDataType="string"/>
+      <xmlPr mapId="2" xpath="/ns1:censusSurveySample/surveyRef" xmlDataType="string"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="6" r="B3" connectionId="0">
+  <singleXmlCell id="2" r="B3" connectionId="0">
     <xmlCellPr id="1" uniqueName="collectionExerciseRef">
-      <xmlPr mapId="1" xpath="/ns1:censusSurveySample/collectionExerciseRef" xmlDataType="string"/>
+      <xmlPr mapId="2" xpath="/ns1:censusSurveySample/collectionExerciseRef" xmlDataType="string"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="7" r="B4" connectionId="0">
+  <singleXmlCell id="3" r="B4" connectionId="0">
     <xmlCellPr id="1" uniqueName="effectiveStartDateTime">
-      <xmlPr mapId="1" xpath="/ns1:censusSurveySample/effectiveStartDateTime" xmlDataType="dateTime"/>
+      <xmlPr mapId="2" xpath="/ns1:censusSurveySample/effectiveStartDateTime" xmlDataType="dateTime"/>
     </xmlCellPr>
   </singleXmlCell>
-  <singleXmlCell id="8" r="B5" connectionId="0">
+  <singleXmlCell id="4" r="B5" connectionId="0">
     <xmlCellPr id="1" uniqueName="effectiveEndDateTime">
-      <xmlPr mapId="1" xpath="/ns1:censusSurveySample/effectiveEndDateTime" xmlDataType="dateTime"/>
+      <xmlPr mapId="2" xpath="/ns1:censusSurveySample/effectiveEndDateTime" xmlDataType="dateTime"/>
     </xmlCellPr>
   </singleXmlCell>
 </singleXmlCells>
@@ -775,7 +828,7 @@
   <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>